<commit_message>
First version of mailing app
</commit_message>
<xml_diff>
--- a/Assets/Client_base.xlsx
+++ b/Assets/Client_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrzom\source\repos\EmailService\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9EB5D5-2A93-4D4A-AEBC-3B8AD07DDE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FF1456-8E91-4641-9231-DC0E3128415C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ФИО</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Почтовый клиент</t>
   </si>
   <si>
-    <t>bidonchik_joe@mail.ru</t>
-  </si>
-  <si>
     <t>Разр Абот Чик</t>
   </si>
   <si>
@@ -73,6 +70,18 @@
   </si>
   <si>
     <t>ivntz.apptest@mail.ru</t>
+  </si>
+  <si>
+    <t>bidonchick_joe@mail.ru</t>
+  </si>
+  <si>
+    <t>Пончик</t>
+  </si>
+  <si>
+    <t>Не пончик</t>
+  </si>
+  <si>
+    <t>ivan_vysotin@bk.ru</t>
   </si>
 </sst>
 </file>
@@ -401,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +474,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>89201002030</v>
@@ -473,25 +482,40 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D5">
         <v>89214005060</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{6A4CD204-11DE-49E5-9952-AAE75F6DEC09}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{29948B1C-8B5D-4F20-B48F-12D316483F0E}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{E660E53F-4DFF-4AE7-B635-F47A6101F8FA}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{00DEFDA2-C810-488B-B31D-048FBCCD672C}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{00DEFDA2-C810-488B-B31D-048FBCCD672C}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{E660E53F-4DFF-4AE7-B635-F47A6101F8FA}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{C168676D-B55E-46A4-B99E-E33346A439BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added path choosing and total mails send
</commit_message>
<xml_diff>
--- a/Assets/Client_base.xlsx
+++ b/Assets/Client_base.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrzom\source\repos\EmailService\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDFEA1E-8F4B-475E-B6D7-2216FCAA62E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA6275-493C-41BF-8B68-6AEAD9176E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>ФИО</t>
   </si>
@@ -57,12 +57,6 @@
     <t>ivntz.apptest.petr@mail.ru</t>
   </si>
   <si>
-    <t>Жо Бидон Амэрикович</t>
-  </si>
-  <si>
-    <t>Почтовый клиент</t>
-  </si>
-  <si>
     <t>Разр Абот Чик</t>
   </si>
   <si>
@@ -72,16 +66,25 @@
     <t>ivntz.apptest@mail.ru</t>
   </si>
   <si>
-    <t>bidonchick_joe@mail.ru</t>
-  </si>
-  <si>
-    <t>Пончик</t>
-  </si>
-  <si>
-    <t>Не пончик</t>
-  </si>
-  <si>
-    <t>ivan.vysotin@list.ru</t>
+    <t>Наименование компании</t>
+  </si>
+  <si>
+    <t>Сбербанк</t>
+  </si>
+  <si>
+    <t>MailRu</t>
+  </si>
+  <si>
+    <t>РЖД</t>
+  </si>
+  <si>
+    <t>ВТБ Банк</t>
+  </si>
+  <si>
+    <t>Клиент почты</t>
+  </si>
+  <si>
+    <t>Василий Иванович Чапаев</t>
   </si>
 </sst>
 </file>
@@ -410,112 +413,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>89123456789</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>89987654321</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>89201002030</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>89201002030</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
+      <c r="E5">
         <v>89214005060</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{6A4CD204-11DE-49E5-9952-AAE75F6DEC09}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{29948B1C-8B5D-4F20-B48F-12D316483F0E}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{00DEFDA2-C810-488B-B31D-048FBCCD672C}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{E660E53F-4DFF-4AE7-B635-F47A6101F8FA}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{C168676D-B55E-46A4-B99E-E33346A439BE}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{6A4CD204-11DE-49E5-9952-AAE75F6DEC09}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{29948B1C-8B5D-4F20-B48F-12D316483F0E}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{00DEFDA2-C810-488B-B31D-048FBCCD672C}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{E660E53F-4DFF-4AE7-B635-F47A6101F8FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Path chose and letter attachment added
</commit_message>
<xml_diff>
--- a/Assets/Client_base.xlsx
+++ b/Assets/Client_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrzom\source\repos\EmailService\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA6275-493C-41BF-8B68-6AEAD9176E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1459F9-F25A-4BD0-B537-1171F391110C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ФИО</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Василий Иванович Чапаев</t>
+  </si>
+  <si>
+    <t>ivntz.apptest.main@mail.ru</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +510,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>89214005060</v>

</xml_diff>

<commit_message>
Table forming partically added
</commit_message>
<xml_diff>
--- a/Assets/Client_base.xlsx
+++ b/Assets/Client_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrzom\source\repos\EmailService\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1459F9-F25A-4BD0-B537-1171F391110C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408D055D-BBCA-4A07-90CC-F9CA2B3B9B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,12 +516,6 @@
         <v>89214005060</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{6A4CD204-11DE-49E5-9952-AAE75F6DEC09}"/>

</xml_diff>